<commit_message>
fixed schedule and added scoreboard alert
</commit_message>
<xml_diff>
--- a/DataGenerator/HYBA-2013Spring-Schedule.xlsx
+++ b/DataGenerator/HYBA-2013Spring-Schedule.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="27">
   <si>
     <t>Michelotti-Red</t>
   </si>
@@ -87,9 +87,6 @@
     <t>Location2Team2</t>
   </si>
   <si>
-    <t>TBD</t>
-  </si>
-  <si>
     <t>TeamName</t>
   </si>
   <si>
@@ -103,6 +100,12 @@
   </si>
   <si>
     <t>Veterans</t>
+  </si>
+  <si>
+    <t>Scoreboard</t>
+  </si>
+  <si>
+    <t>Location2Scoreboard</t>
   </si>
 </sst>
 </file>
@@ -126,7 +129,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -136,6 +139,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -161,19 +170,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,22 +466,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="19.5703125" customWidth="1"/>
-    <col min="6" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="19.5703125" customWidth="1"/>
+    <col min="7" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -483,20 +493,25 @@
         <v>4</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" s="3"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>41383</v>
       </c>
@@ -510,20 +525,14 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" t="s">
         <v>24</v>
       </c>
-      <c r="F2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="4"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="4"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>41383</v>
       </c>
@@ -537,20 +546,20 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" t="s">
         <v>24</v>
       </c>
-      <c r="F3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="4"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="4"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>41383</v>
       </c>
@@ -564,157 +573,162 @@
         <v>15</v>
       </c>
       <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" t="s">
         <v>24</v>
       </c>
-      <c r="F4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" s="4"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
         <v>41383</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="6">
         <v>0.375</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="9" t="s">
+      <c r="J5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="4"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>41390</v>
       </c>
       <c r="B6" s="2">
         <v>0.25</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="13" t="s">
         <v>17</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
       </c>
       <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="9"/>
+      <c r="I6" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" s="4"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="4"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>41390</v>
       </c>
       <c r="B7" s="2">
         <v>0.29166666666666669</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>16</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
       </c>
       <c r="E7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I7" s="4"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" s="4"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>41390</v>
       </c>
       <c r="B8" s="2">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D8" t="s">
         <v>13</v>
       </c>
       <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" t="s">
-        <v>25</v>
-      </c>
-      <c r="I8" s="4"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
         <v>41390</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <v>0.375</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="J9" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="I9" s="4"/>
     </row>
   </sheetData>
-  <sortState ref="I2:I15">
-    <sortCondition ref="I2:I15"/>
+  <sortState ref="J2:J15">
+    <sortCondition ref="J2:J15"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -736,7 +750,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -744,7 +758,7 @@
         <v>15</v>
       </c>
       <c r="B2">
-        <f>COUNTIF(Games!$C$2:$G$9, Teams!A2)</f>
+        <f>COUNTIF(Games!$C$2:$H$9, Teams!A2)</f>
         <v>2</v>
       </c>
     </row>
@@ -753,8 +767,8 @@
         <v>17</v>
       </c>
       <c r="B3">
-        <f>COUNTIF(Games!$C$2:$G$9, Teams!A3)</f>
-        <v>2</v>
+        <f>COUNTIF(Games!$C$2:$H$9, Teams!A3)</f>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -762,7 +776,7 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <f>COUNTIF(Games!$C$2:$G$9, Teams!A4)</f>
+        <f>COUNTIF(Games!$C$2:$H$9, Teams!A4)</f>
         <v>2</v>
       </c>
     </row>
@@ -771,7 +785,7 @@
         <v>12</v>
       </c>
       <c r="B5">
-        <f>COUNTIF(Games!$C$2:$G$9, Teams!A5)</f>
+        <f>COUNTIF(Games!$C$2:$H$9, Teams!A5)</f>
         <v>2</v>
       </c>
     </row>
@@ -780,7 +794,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <f>COUNTIF(Games!$C$2:$G$9, Teams!A6)</f>
+        <f>COUNTIF(Games!$C$2:$H$9, Teams!A6)</f>
         <v>2</v>
       </c>
     </row>
@@ -789,7 +803,7 @@
         <v>0</v>
       </c>
       <c r="B7">
-        <f>COUNTIF(Games!$C$2:$G$9, Teams!A7)</f>
+        <f>COUNTIF(Games!$C$2:$H$9, Teams!A7)</f>
         <v>2</v>
       </c>
     </row>
@@ -798,7 +812,7 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <f>COUNTIF(Games!$C$2:$G$9, Teams!A8)</f>
+        <f>COUNTIF(Games!$C$2:$H$9, Teams!A8)</f>
         <v>2</v>
       </c>
     </row>
@@ -807,7 +821,7 @@
         <v>16</v>
       </c>
       <c r="B9">
-        <f>COUNTIF(Games!$C$2:$G$9, Teams!A9)</f>
+        <f>COUNTIF(Games!$C$2:$H$9, Teams!A9)</f>
         <v>2</v>
       </c>
     </row>
@@ -816,7 +830,7 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <f>COUNTIF(Games!$C$2:$G$9, Teams!A10)</f>
+        <f>COUNTIF(Games!$C$2:$H$9, Teams!A10)</f>
         <v>2</v>
       </c>
     </row>
@@ -825,7 +839,7 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <f>COUNTIF(Games!$C$2:$G$9, Teams!A11)</f>
+        <f>COUNTIF(Games!$C$2:$H$9, Teams!A11)</f>
         <v>2</v>
       </c>
     </row>
@@ -834,7 +848,7 @@
         <v>6</v>
       </c>
       <c r="B12">
-        <f>COUNTIF(Games!$C$2:$G$9, Teams!A12)</f>
+        <f>COUNTIF(Games!$C$2:$H$9, Teams!A12)</f>
         <v>2</v>
       </c>
     </row>
@@ -843,8 +857,8 @@
         <v>7</v>
       </c>
       <c r="B13">
-        <f>COUNTIF(Games!$C$2:$G$9, Teams!A13)</f>
-        <v>2</v>
+        <f>COUNTIF(Games!$C$2:$H$9, Teams!A13)</f>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -852,7 +866,7 @@
         <v>10</v>
       </c>
       <c r="B14">
-        <f>COUNTIF(Games!$C$2:$G$9, Teams!A14)</f>
+        <f>COUNTIF(Games!$C$2:$H$9, Teams!A14)</f>
         <v>2</v>
       </c>
     </row>
@@ -861,7 +875,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <f>COUNTIF(Games!$C$2:$G$9, Teams!A15)</f>
+        <f>COUNTIF(Games!$C$2:$H$9, Teams!A15)</f>
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added exception at Centennial
</commit_message>
<xml_diff>
--- a/DataGenerator/HYBA-2013Spring-Schedule.xlsx
+++ b/DataGenerator/HYBA-2013Spring-Schedule.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="55">
   <si>
     <t>Michelotti-Red</t>
   </si>
@@ -193,6 +193,9 @@
   </si>
   <si>
     <t>2v3</t>
+  </si>
+  <si>
+    <t>Centennial-HS</t>
   </si>
 </sst>
 </file>
@@ -755,7 +758,7 @@
   <dimension ref="A1:Q37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,6 +767,7 @@
     <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="19.5703125" customWidth="1"/>
     <col min="7" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1241,7 +1245,7 @@
       </c>
       <c r="F14" s="21"/>
       <c r="I14" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="J14" s="21"/>
       <c r="Q14" t="s">
@@ -1272,7 +1276,7 @@
         <v>7</v>
       </c>
       <c r="I15" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="J15" s="21"/>
       <c r="L15" t="s">
@@ -1309,7 +1313,7 @@
         <v>11</v>
       </c>
       <c r="I16" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="J16" s="21"/>
       <c r="L16" t="s">
@@ -1343,7 +1347,7 @@
         <v>12</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="J17" s="23" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
added Long Reach HS locations
</commit_message>
<xml_diff>
--- a/DataGenerator/HYBA-2013Spring-Schedule.xlsx
+++ b/DataGenerator/HYBA-2013Spring-Schedule.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="56">
   <si>
     <t>Michelotti-Red</t>
   </si>
@@ -196,6 +196,9 @@
   </si>
   <si>
     <t>Centennial-HS</t>
+  </si>
+  <si>
+    <t>Long-Reach-HS</t>
   </si>
 </sst>
 </file>
@@ -755,10 +758,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q37"/>
+  <dimension ref="A1:Q33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1503,7 +1506,7 @@
       </c>
       <c r="F22" s="21"/>
       <c r="I22" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="J22" s="21"/>
     </row>
@@ -1531,7 +1534,7 @@
         <v>9</v>
       </c>
       <c r="I23" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="J23" s="21"/>
       <c r="L23" t="s">
@@ -1565,7 +1568,7 @@
         <v>11</v>
       </c>
       <c r="I24" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="J24" s="21"/>
       <c r="L24" t="s">
@@ -1599,7 +1602,7 @@
         <v>7</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="J25" s="23" t="s">
         <v>14</v>
@@ -1618,14 +1621,16 @@
       <c r="B26" s="18">
         <v>0.25</v>
       </c>
-      <c r="C26" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="D26" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="E26" s="36"/>
-      <c r="F26" s="37"/>
+      <c r="C26" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" t="s">
+        <v>55</v>
+      </c>
+      <c r="F26" s="21"/>
       <c r="I26" t="s">
         <v>21</v>
       </c>
@@ -1638,14 +1643,16 @@
       <c r="B27" s="18">
         <v>0.29166666666666669</v>
       </c>
-      <c r="C27" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="D27" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="E27" s="36"/>
-      <c r="F27" s="37"/>
+      <c r="C27" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E27" t="s">
+        <v>55</v>
+      </c>
+      <c r="F27" s="21"/>
       <c r="G27" t="s">
         <v>9</v>
       </c>
@@ -1670,14 +1677,16 @@
       <c r="B28" s="18">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C28" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="D28" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="E28" s="36"/>
-      <c r="F28" s="37"/>
+      <c r="C28" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" t="s">
+        <v>55</v>
+      </c>
+      <c r="F28" s="21"/>
       <c r="G28" t="s">
         <v>13</v>
       </c>
@@ -1702,14 +1711,16 @@
       <c r="B29" s="19">
         <v>0.375</v>
       </c>
-      <c r="C29" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="D29" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="E29" s="38"/>
-      <c r="F29" s="39"/>
+      <c r="C29" s="66" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F29" s="23"/>
       <c r="G29" s="66" t="s">
         <v>8</v>
       </c>
@@ -1737,10 +1748,10 @@
         <v>0.25</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" s="7" t="s">
         <v>26</v>
+      </c>
+      <c r="D30" s="69" t="s">
+        <v>7</v>
       </c>
       <c r="E30" t="s">
         <v>20</v>
@@ -1759,7 +1770,7 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>25</v>
@@ -1792,11 +1803,11 @@
       <c r="B32" s="18">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C32" s="40" t="s">
+      <c r="C32" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D32" s="7" t="s">
         <v>6</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>10</v>
       </c>
       <c r="E32" t="s">
         <v>20</v>
@@ -1826,16 +1837,18 @@
       <c r="B33" s="19">
         <v>0.375</v>
       </c>
-      <c r="C33" s="66" t="s">
-        <v>7</v>
+      <c r="C33" s="8" t="s">
+        <v>0</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F33" s="23"/>
+      <c r="F33" s="23" t="s">
+        <v>0</v>
+      </c>
       <c r="G33" s="64" t="s">
         <v>14</v>
       </c>
@@ -1854,112 +1867,6 @@
       <c r="M33" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="12">
-        <v>41439</v>
-      </c>
-      <c r="B34" s="18">
-        <v>0.25</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D34" s="69" t="s">
-        <v>7</v>
-      </c>
-      <c r="E34" t="s">
-        <v>20</v>
-      </c>
-      <c r="F34" s="21"/>
-      <c r="G34" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="H34" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="I34" s="36"/>
-      <c r="J34" s="37"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="12">
-        <v>41439</v>
-      </c>
-      <c r="B35" s="18">
-        <v>0.29166666666666669</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E35" t="s">
-        <v>20</v>
-      </c>
-      <c r="F35" s="21"/>
-      <c r="G35" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="H35" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="I35" s="36"/>
-      <c r="J35" s="37"/>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="12">
-        <v>41439</v>
-      </c>
-      <c r="B36" s="18">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E36" t="s">
-        <v>20</v>
-      </c>
-      <c r="F36" s="21"/>
-      <c r="G36" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="H36" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="I36" s="36"/>
-      <c r="J36" s="37"/>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="13">
-        <v>41439</v>
-      </c>
-      <c r="B37" s="19">
-        <v>0.375</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F37" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="G37" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="H37" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="I37" s="38"/>
-      <c r="J37" s="39"/>
     </row>
   </sheetData>
   <sortState ref="J2:J15">

</xml_diff>

<commit_message>
week #7 location changes
</commit_message>
<xml_diff>
--- a/DataGenerator/HYBA-2013Spring-Schedule.xlsx
+++ b/DataGenerator/HYBA-2013Spring-Schedule.xlsx
@@ -761,7 +761,7 @@
   <dimension ref="A1:Q33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1628,11 +1628,11 @@
         <v>26</v>
       </c>
       <c r="E26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F26" s="21"/>
       <c r="I26" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="J26" s="21"/>
     </row>
@@ -1650,7 +1650,7 @@
         <v>25</v>
       </c>
       <c r="E27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F27" s="21"/>
       <c r="G27" t="s">
@@ -1660,7 +1660,7 @@
         <v>14</v>
       </c>
       <c r="I27" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="J27" s="21"/>
       <c r="L27" t="s">
@@ -1684,7 +1684,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F28" s="21"/>
       <c r="G28" t="s">
@@ -1694,7 +1694,7 @@
         <v>12</v>
       </c>
       <c r="I28" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="J28" s="21"/>
       <c r="L28" t="s">
@@ -1718,7 +1718,7 @@
         <v>29</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F29" s="23"/>
       <c r="G29" s="66" t="s">
@@ -1728,7 +1728,7 @@
         <v>11</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="J29" s="23" t="s">
         <v>8</v>

</xml_diff>